<commit_message>
differentiated the criteria for identifying if the test case was pass or fail, changed the assertion statement accordin to the test case
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -515,16 +515,16 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>8.630000000000001</v>
+        <v>7.38</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-03-07 01:52:25</t>
+          <t>2025-03-07 02:36:17</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2025-03-07 01:52:34</t>
+          <t>2025-03-07 02:36:24</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -562,7 +562,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>User gets Welcome Username in the Dropdown</t>
+          <t>User is redirected to their account page after login</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -571,16 +571,16 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>5.33</v>
+        <v>7.33</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-03-07 01:52:38</t>
+          <t>2025-03-07 02:36:28</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2025-03-07 01:52:43</t>
+          <t>2025-03-07 02:36:35</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">

</xml_diff>

<commit_message>
Added BDD support using pytest-bdd
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -515,16 +515,16 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>8.109999999999999</v>
+        <v>0.02</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-03-07 02:39:13</t>
+          <t>2025-03-10 18:29:39</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2025-03-07 02:39:21</t>
+          <t>2025-03-10 18:29:39</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -571,16 +571,16 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>8.07</v>
+        <v>1.03</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-03-07 02:39:25</t>
+          <t>2025-03-10 18:29:49</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2025-03-07 02:39:33</t>
+          <t>2025-03-10 18:29:50</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">

</xml_diff>

<commit_message>
Added BDD version recording
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -515,16 +515,16 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-03-10 18:29:39</t>
+          <t>2025-03-10 18:36:12</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2025-03-10 18:29:39</t>
+          <t>2025-03-10 18:36:12</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -575,12 +575,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-03-10 18:29:49</t>
+          <t>2025-03-10 18:36:21</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2025-03-10 18:29:50</t>
+          <t>2025-03-10 18:36:22</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">

</xml_diff>